<commit_message>
Added screenshot for nexus
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/Signature_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/Signature_JS.xlsx
@@ -718,36 +718,6 @@
 validate1;
 link_Click(signature_test_link);
 validate2;
-SelectTestToRun(VT200_0885_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-Rotate_Screen(landscape);
-wait(2);
-TakeScreenshot(VT200-0885);
-wait(2);
-validate4;</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-link_Click(signature_test_link);
-validate2;
-SelectTestToRun(VT200_0886_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-Rotate_Screen(landscape);
-wait(2);
-TakeScreenshot(VT200-0886);
-wait(2);
-validate4;</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-link_Click(signature_test_link);
-validate2;
 SelectTestToRun(VT200_0887_string);
 ClickRunTest(runtest_top_xpath);
 validate3;
@@ -799,6 +769,38 @@
 TakeScreenshot(VT200-0893-02);
 wait(2);
 validate4;</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(signature_test_link);
+validate2;
+SelectTestToRun(VT200_0885_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+Rotate_Screen(landscape);
+wait(2);
+TakeScreenshot(VT200-0885);
+wait(2);
+validate4;
+Rotate_Screen(potrait);</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(signature_test_link);
+validate2;
+SelectTestToRun(VT200_0886_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+Rotate_Screen(landscape);
+wait(2);
+TakeScreenshot(VT200-0886);
+wait(2);
+validate4;
+Rotate_Screen(potrait);</t>
   </si>
 </sst>
 </file>
@@ -1388,7 +1390,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1701,7 +1703,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>33</v>
@@ -1726,7 +1728,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>34</v>
@@ -1751,7 +1753,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>35</v>
@@ -1803,7 +1805,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>56</v>
@@ -1903,7 +1905,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>40</v>

</xml_diff>